<commit_message>
Scrapper ready for production
</commit_message>
<xml_diff>
--- a/CATI/saved_states/CHCL_future_30_day_forecast.xlsx
+++ b/CATI/saved_states/CHCL_future_30_day_forecast.xlsx
@@ -456,7 +456,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45919</v>
+        <v>45940</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -464,12 +464,12 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.289630675689082</v>
+        <v>0.2660646151183387</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45922</v>
+        <v>45943</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -477,12 +477,12 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.2946104026090812</v>
+        <v>0.2574717995054228</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45923</v>
+        <v>45944</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -490,12 +490,12 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.2134914762031745</v>
+        <v>0.2493119621046376</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45924</v>
+        <v>45945</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -503,12 +503,12 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.173970631386013</v>
+        <v>0.2336090690140274</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45925</v>
+        <v>45946</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -516,12 +516,12 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1352373874437522</v>
+        <v>0.2349794051493647</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45926</v>
+        <v>45947</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -529,12 +529,12 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.1023256099474144</v>
+        <v>0.2330001286114695</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45929</v>
+        <v>45950</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -542,12 +542,12 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.07825447532054898</v>
+        <v>0.2344442068268122</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45930</v>
+        <v>45951</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -555,12 +555,12 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.07408778282520291</v>
+        <v>0.2359496702182244</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45931</v>
+        <v>45952</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -568,12 +568,12 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.06950184243437764</v>
+        <v>0.2283995496571739</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45932</v>
+        <v>45953</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -581,12 +581,12 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.06958587008234975</v>
+        <v>0.2251089505700687</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45933</v>
+        <v>45954</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -594,12 +594,12 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.07083008832402647</v>
+        <v>0.2234114996938327</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45936</v>
+        <v>45957</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -607,12 +607,12 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.07232818028994024</v>
+        <v>0.2223929684345076</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45937</v>
+        <v>45958</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -620,12 +620,12 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.07355943716235579</v>
+        <v>0.2291202871244187</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45938</v>
+        <v>45959</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -633,12 +633,12 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.0748082028991741</v>
+        <v>0.2319713214561409</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45939</v>
+        <v>45960</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -646,12 +646,12 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.07526775471039236</v>
+        <v>0.2338585535213417</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45940</v>
+        <v>45961</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -659,12 +659,12 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.07538710556097449</v>
+        <v>0.2315027899831548</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45943</v>
+        <v>45964</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -672,12 +672,12 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.07634482554264486</v>
+        <v>0.2335542066693475</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45944</v>
+        <v>45965</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -685,12 +685,12 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.07751949525542677</v>
+        <v>0.235117210053213</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45945</v>
+        <v>45966</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -698,12 +698,12 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.07878522223897398</v>
+        <v>0.2351532779527054</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45946</v>
+        <v>45967</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -711,12 +711,12 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.07985904834337652</v>
+        <v>0.2429966940770025</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45947</v>
+        <v>45968</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -724,12 +724,12 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.08113096303410948</v>
+        <v>0.2423682593055715</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45950</v>
+        <v>45971</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -737,12 +737,12 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.08224697097953609</v>
+        <v>0.2436330769571086</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45951</v>
+        <v>45972</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -750,12 +750,12 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.08315766289647869</v>
+        <v>0.2633896615943274</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45952</v>
+        <v>45973</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -763,12 +763,12 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.08427061572488598</v>
+        <v>0.2655242454178919</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -776,12 +776,12 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.08546000778492741</v>
+        <v>0.2664659839041819</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45954</v>
+        <v>45975</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -789,12 +789,12 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.08627189143143302</v>
+        <v>0.2609385276189906</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45957</v>
+        <v>45978</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -802,12 +802,12 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.08647106780253058</v>
+        <v>0.2586563026622665</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45958</v>
+        <v>45979</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -815,12 +815,12 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.08689369453631049</v>
+        <v>0.2612144140843821</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45959</v>
+        <v>45980</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -828,12 +828,12 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.08740897296510344</v>
+        <v>0.2670336621723229</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45960</v>
+        <v>45981</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -841,7 +841,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.08898574760176736</v>
+        <v>0.2622518556396169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>